<commit_message>
add edit family maseter
</commit_message>
<xml_diff>
--- a/docs/churchcrm.xlsx
+++ b/docs/churchcrm.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Done" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="49">
   <si>
     <t>routing</t>
   </si>
@@ -137,6 +137,33 @@
   </si>
   <si>
     <t>exporting</t>
+  </si>
+  <si>
+    <t>add new year in Admin menu</t>
+  </si>
+  <si>
+    <t>churchcrm</t>
+  </si>
+  <si>
+    <t>newYearEditor.php</t>
+  </si>
+  <si>
+    <t>creating file</t>
+  </si>
+  <si>
+    <t>adding new menu item</t>
+  </si>
+  <si>
+    <t>adding new year</t>
+  </si>
+  <si>
+    <t>menu.php</t>
+  </si>
+  <si>
+    <t>add file for  new year in Admin menu</t>
+  </si>
+  <si>
+    <t>adding new year button</t>
   </si>
 </sst>
 </file>
@@ -214,7 +241,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -247,6 +274,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -552,16 +582,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AN28"/>
+  <dimension ref="A1:AN36"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="30.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="34.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="2" style="5" customWidth="1"/>
     <col min="6" max="6" width="16.44140625" bestFit="1" customWidth="1"/>
@@ -575,7 +605,7 @@
       <c r="B1" s="4"/>
     </row>
     <row r="2" spans="1:10" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="13" t="s">
         <v>20</v>
       </c>
       <c r="B2" s="6">
@@ -591,7 +621,7 @@
       <c r="H2"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A3" s="3"/>
+      <c r="A3" s="13"/>
       <c r="B3" s="11" t="s">
         <v>7</v>
       </c>
@@ -608,7 +638,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="3"/>
+      <c r="A4" s="13"/>
       <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
@@ -634,16 +664,16 @@
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="3"/>
+      <c r="A5" s="13"/>
       <c r="E5"/>
       <c r="H5"/>
     </row>
     <row r="6" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3"/>
+      <c r="A6" s="13"/>
       <c r="B6" s="4"/>
     </row>
     <row r="7" spans="1:10" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A7" s="3"/>
+      <c r="A7" s="13"/>
       <c r="B7" s="6">
         <v>2</v>
       </c>
@@ -655,7 +685,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="3"/>
+      <c r="A8" s="13"/>
       <c r="B8" s="11" t="s">
         <v>16</v>
       </c>
@@ -664,7 +694,7 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="3"/>
+      <c r="A9" s="13"/>
       <c r="B9" s="2" t="s">
         <v>15</v>
       </c>
@@ -676,17 +706,17 @@
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="3"/>
+      <c r="A10" s="13"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="3"/>
+      <c r="A11" s="13"/>
     </row>
     <row r="12" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="3"/>
+      <c r="A12" s="13"/>
       <c r="B12" s="4"/>
     </row>
     <row r="13" spans="1:10" ht="19.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="3"/>
+      <c r="A13" s="13"/>
       <c r="B13" s="6">
         <v>3</v>
       </c>
@@ -698,7 +728,7 @@
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A14" s="3"/>
+      <c r="A14" s="13"/>
       <c r="B14" s="11" t="s">
         <v>16</v>
       </c>
@@ -707,7 +737,7 @@
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="3"/>
+      <c r="A15" s="13"/>
       <c r="B15" s="2" t="s">
         <v>18</v>
       </c>
@@ -715,224 +745,292 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="B16"/>
-    </row>
-    <row r="17" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="4"/>
-    </row>
-    <row r="18" spans="1:40" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A18" s="1" t="s">
+    <row r="16" spans="1:10" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="3"/>
+      <c r="B16" s="4"/>
+    </row>
+    <row r="17" spans="1:40" ht="19.8" x14ac:dyDescent="0.3">
+      <c r="A17" s="3"/>
+      <c r="B17" s="6">
+        <v>4</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="A18" s="3"/>
+      <c r="B18" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="3"/>
+      <c r="B20" s="4"/>
+    </row>
+    <row r="21" spans="1:40" ht="19.8" x14ac:dyDescent="0.3">
+      <c r="A21" s="3"/>
+      <c r="B21" s="6">
+        <v>5</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D21" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="A22" s="3"/>
+      <c r="B22" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="B24"/>
+    </row>
+    <row r="25" spans="1:40" s="5" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B25" s="4"/>
+    </row>
+    <row r="26" spans="1:40" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="A26" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B18" s="6">
-        <v>4</v>
-      </c>
-      <c r="C18" s="7" t="s">
+      <c r="B26" s="6">
         <v>1</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="A19" s="1"/>
-      <c r="B19" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C19" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:40" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A20" s="1"/>
-      <c r="B20" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D20" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E20" s="8"/>
-      <c r="H20" s="8"/>
-    </row>
-    <row r="21" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="A21" s="1"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="4"/>
-      <c r="M21" s="4"/>
-      <c r="N21" s="4"/>
-      <c r="O21" s="4"/>
-      <c r="P21" s="4"/>
-      <c r="Q21" s="4"/>
-      <c r="R21" s="4"/>
-      <c r="S21" s="4"/>
-      <c r="T21" s="4"/>
-      <c r="U21" s="4"/>
-      <c r="V21" s="4"/>
-      <c r="W21" s="4"/>
-      <c r="X21" s="4"/>
-      <c r="Y21" s="4"/>
-      <c r="Z21" s="4"/>
-      <c r="AA21" s="4"/>
-      <c r="AB21" s="4"/>
-      <c r="AC21" s="4"/>
-      <c r="AD21" s="4"/>
-      <c r="AE21" s="4"/>
-      <c r="AF21" s="4"/>
-      <c r="AG21" s="4"/>
-      <c r="AH21" s="4"/>
-      <c r="AI21" s="4"/>
-      <c r="AJ21" s="4"/>
-      <c r="AK21" s="4"/>
-      <c r="AL21" s="4"/>
-      <c r="AM21" s="4"/>
-      <c r="AN21" s="4"/>
-    </row>
-    <row r="22" spans="1:40" s="5" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
-      <c r="A22" s="1"/>
-      <c r="B22" s="6">
-        <v>5</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="F22"/>
-      <c r="G22"/>
-      <c r="I22"/>
-      <c r="J22"/>
-      <c r="K22"/>
-      <c r="L22"/>
-      <c r="M22"/>
-      <c r="N22"/>
-      <c r="O22"/>
-      <c r="P22"/>
-      <c r="Q22"/>
-      <c r="R22"/>
-      <c r="S22"/>
-      <c r="T22"/>
-      <c r="U22"/>
-    </row>
-    <row r="23" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="A23" s="1"/>
-      <c r="B23" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C23" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:40" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="1"/>
-      <c r="B24" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:40" x14ac:dyDescent="0.3">
-      <c r="A25" s="1"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="4"/>
-      <c r="J25" s="4"/>
-      <c r="K25" s="4"/>
-      <c r="L25" s="4"/>
-      <c r="M25" s="4"/>
-      <c r="N25" s="4"/>
-      <c r="O25" s="4"/>
-      <c r="P25" s="4"/>
-      <c r="Q25" s="4"/>
-      <c r="R25" s="4"/>
-      <c r="S25" s="4"/>
-      <c r="T25" s="4"/>
-      <c r="U25" s="4"/>
-      <c r="V25" s="4"/>
-      <c r="W25" s="4"/>
-      <c r="X25" s="4"/>
-      <c r="Y25" s="4"/>
-      <c r="Z25" s="4"/>
-      <c r="AA25" s="4"/>
-      <c r="AB25" s="4"/>
-      <c r="AC25" s="4"/>
-      <c r="AD25" s="4"/>
-      <c r="AE25" s="4"/>
-      <c r="AF25" s="4"/>
-      <c r="AG25" s="4"/>
-      <c r="AH25" s="4"/>
-      <c r="AI25" s="4"/>
-      <c r="AJ25" s="4"/>
-      <c r="AK25" s="4"/>
-      <c r="AL25" s="4"/>
-      <c r="AM25" s="4"/>
-      <c r="AN25" s="4"/>
-    </row>
-    <row r="26" spans="1:40" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.4">
-      <c r="A26" s="1"/>
-      <c r="B26" s="6">
-        <v>6</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="D26" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="F26"/>
-      <c r="G26"/>
-      <c r="I26"/>
-      <c r="J26"/>
-      <c r="K26"/>
-      <c r="L26"/>
-      <c r="M26"/>
-      <c r="N26"/>
-      <c r="O26"/>
-      <c r="P26"/>
-      <c r="Q26"/>
-      <c r="R26"/>
-      <c r="S26"/>
-      <c r="T26"/>
-      <c r="U26"/>
+      <c r="D26" s="10" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="27" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="A27" s="1"/>
       <c r="B27" s="11" t="s">
         <v>16</v>
       </c>
       <c r="C27" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:40" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A28" s="1"/>
+      <c r="B28" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D28" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E28" s="8"/>
+      <c r="H28" s="8"/>
+    </row>
+    <row r="29" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="A29" s="1"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="4"/>
+      <c r="M29" s="4"/>
+      <c r="N29" s="4"/>
+      <c r="O29" s="4"/>
+      <c r="P29" s="4"/>
+      <c r="Q29" s="4"/>
+      <c r="R29" s="4"/>
+      <c r="S29" s="4"/>
+      <c r="T29" s="4"/>
+      <c r="U29" s="4"/>
+      <c r="V29" s="4"/>
+      <c r="W29" s="4"/>
+      <c r="X29" s="4"/>
+      <c r="Y29" s="4"/>
+      <c r="Z29" s="4"/>
+      <c r="AA29" s="4"/>
+      <c r="AB29" s="4"/>
+      <c r="AC29" s="4"/>
+      <c r="AD29" s="4"/>
+      <c r="AE29" s="4"/>
+      <c r="AF29" s="4"/>
+      <c r="AG29" s="4"/>
+      <c r="AH29" s="4"/>
+      <c r="AI29" s="4"/>
+      <c r="AJ29" s="4"/>
+      <c r="AK29" s="4"/>
+      <c r="AL29" s="4"/>
+      <c r="AM29" s="4"/>
+      <c r="AN29" s="4"/>
+    </row>
+    <row r="30" spans="1:40" s="5" customFormat="1" ht="19.8" x14ac:dyDescent="0.4">
+      <c r="A30" s="1"/>
+      <c r="B30" s="6">
+        <v>2</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D30" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="F30"/>
+      <c r="G30"/>
+      <c r="I30"/>
+      <c r="J30"/>
+      <c r="K30"/>
+      <c r="L30"/>
+      <c r="M30"/>
+      <c r="N30"/>
+      <c r="O30"/>
+      <c r="P30"/>
+      <c r="Q30"/>
+      <c r="R30"/>
+      <c r="S30"/>
+      <c r="T30"/>
+      <c r="U30"/>
+    </row>
+    <row r="31" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="A31" s="1"/>
+      <c r="B31" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C31" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:40" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B28" s="9" t="s">
+    <row r="32" spans="1:40" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="1"/>
+      <c r="B32" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="A33" s="1"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="4"/>
+      <c r="J33" s="4"/>
+      <c r="K33" s="4"/>
+      <c r="L33" s="4"/>
+      <c r="M33" s="4"/>
+      <c r="N33" s="4"/>
+      <c r="O33" s="4"/>
+      <c r="P33" s="4"/>
+      <c r="Q33" s="4"/>
+      <c r="R33" s="4"/>
+      <c r="S33" s="4"/>
+      <c r="T33" s="4"/>
+      <c r="U33" s="4"/>
+      <c r="V33" s="4"/>
+      <c r="W33" s="4"/>
+      <c r="X33" s="4"/>
+      <c r="Y33" s="4"/>
+      <c r="Z33" s="4"/>
+      <c r="AA33" s="4"/>
+      <c r="AB33" s="4"/>
+      <c r="AC33" s="4"/>
+      <c r="AD33" s="4"/>
+      <c r="AE33" s="4"/>
+      <c r="AF33" s="4"/>
+      <c r="AG33" s="4"/>
+      <c r="AH33" s="4"/>
+      <c r="AI33" s="4"/>
+      <c r="AJ33" s="4"/>
+      <c r="AK33" s="4"/>
+      <c r="AL33" s="4"/>
+      <c r="AM33" s="4"/>
+      <c r="AN33" s="4"/>
+    </row>
+    <row r="34" spans="1:40" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.4">
+      <c r="A34" s="1"/>
+      <c r="B34" s="6">
+        <v>3</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D34" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="F34"/>
+      <c r="G34"/>
+      <c r="I34"/>
+      <c r="J34"/>
+      <c r="K34"/>
+      <c r="L34"/>
+      <c r="M34"/>
+      <c r="N34"/>
+      <c r="O34"/>
+      <c r="P34"/>
+      <c r="Q34"/>
+      <c r="R34"/>
+      <c r="S34"/>
+      <c r="T34"/>
+      <c r="U34"/>
+    </row>
+    <row r="35" spans="1:40" x14ac:dyDescent="0.3">
+      <c r="B35" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="C35" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="36" spans="1:40" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B36" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C28" s="2" t="s">
+      <c r="C36" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D28" s="9" t="s">
+      <c r="D36" s="9" t="s">
         <v>34</v>
       </c>
     </row>
@@ -949,7 +1047,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>

</xml_diff>